<commit_message>
Updating about the authors and dcf output
</commit_message>
<xml_diff>
--- a/DCF Excel/DCF.xlsx
+++ b/DCF Excel/DCF.xlsx
@@ -5,18 +5,19 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a0eb7a0542c45fb0/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\niamh\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="212" documentId="8_{3B34180D-096B-48E4-8BEC-843F98F05358}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2ED47EA6-3A5E-433F-BB9D-57B3F86D0032}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FA13E8F-12F1-49A0-BC97-E162CB410918}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{02DDE7C9-D2BD-4C78-80A5-9CD0E38E0A7F}"/>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{A124F699-F544-4474-B589-20D8B152A358}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="2" xr2:uid="{02DDE7C9-D2BD-4C78-80A5-9CD0E38E0A7F}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{A124F699-F544-4474-B589-20D8B152A358}"/>
   </bookViews>
   <sheets>
-    <sheet name="Cover Page " sheetId="4" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Front page table" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="5" r:id="rId1"/>
+    <sheet name="Cover Page " sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet5" sheetId="2" r:id="rId3"/>
+    <sheet name="Front page table" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="61">
   <si>
     <t>ENTERPRISE VALUE CALCULATION</t>
   </si>
@@ -400,7 +401,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -444,6 +445,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -778,115 +780,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AA70213-F3C2-4630-B34B-890FBA1251F3}">
-  <dimension ref="A1:D5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D395B51-2BB7-401F-ABD9-7600F8F8CFD4}">
+  <dimension ref="A1:O26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E4"/>
+    <sheetView topLeftCell="A4" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="88" workbookViewId="1">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="26.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.06640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B2">
-        <v>4.2</v>
-      </c>
-      <c r="C2">
-        <v>1.8</v>
-      </c>
-      <c r="D2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B3">
-        <v>3.5</v>
-      </c>
-      <c r="C3">
-        <v>1.5</v>
-      </c>
-      <c r="D3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B4">
-        <v>4.5</v>
-      </c>
-      <c r="C4">
-        <v>1.8</v>
-      </c>
-      <c r="D4">
-        <v>6.3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B5">
-        <v>4.7</v>
-      </c>
-      <c r="C5">
-        <v>0.6</v>
-      </c>
-      <c r="D5">
-        <v>5.3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5393FF5A-4A4F-4A89-8BF1-96F397853368}">
-  <dimension ref="A1:O26"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="63" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
-    </sheetView>
-    <sheetView topLeftCell="A4" zoomScale="88" workbookViewId="1">
-      <selection activeCell="D20" sqref="D20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.08984375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -906,7 +817,7 @@
         <v>2029</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -926,7 +837,7 @@
         <v>871</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -946,7 +857,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -966,7 +877,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -991,22 +902,21 @@
         <v>606.70256877695113</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="16.5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" ht="16.5" x14ac:dyDescent="0.6">
       <c r="A9" s="22" t="s">
         <v>0</v>
       </c>
       <c r="B9" s="23"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B10" s="4">
-        <f>F2</f>
         <v>871</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11" s="3" t="s">
         <v>60</v>
       </c>
@@ -1014,13 +924,12 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A12" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="6">
-        <f>B10*(1+B11)</f>
-        <v>892.77499999999998</v>
+      <c r="B12" s="29">
+        <v>893</v>
       </c>
       <c r="F12" s="19" t="s">
         <v>6</v>
@@ -1030,16 +939,15 @@
       </c>
       <c r="H12" s="16">
         <f>B16</f>
-        <v>15541.170416178069</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+        <v>15545</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A13" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B13" s="4">
-        <f>B12/(F3-B11)</f>
-        <v>17855.5</v>
+        <v>17860</v>
       </c>
       <c r="F13" s="19" t="s">
         <v>36</v>
@@ -1052,13 +960,12 @@
         <v>6262</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A14" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B14" s="4">
-        <f>B13/(1+F3)^F4</f>
-        <v>12437.402659927498</v>
+        <v>12441</v>
       </c>
       <c r="F14" s="19" t="s">
         <v>10</v>
@@ -1068,16 +975,15 @@
       </c>
       <c r="H14" s="16">
         <f>B20</f>
-        <v>9279.170416178069</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+        <v>9283</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B15" s="4">
-        <f>SUM(B5:F5)</f>
-        <v>3103.7677562505714</v>
+        <v>3104</v>
       </c>
       <c r="F15" s="19" t="s">
         <v>38</v>
@@ -1090,13 +996,12 @@
         <v>1853</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A16" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B16" s="8">
-        <f>SUM(B14:B15)</f>
-        <v>15541.170416178069</v>
+        <v>15545</v>
       </c>
       <c r="F16" s="19" t="s">
         <v>39</v>
@@ -1106,21 +1011,21 @@
       </c>
       <c r="H16" s="18">
         <f>B24</f>
-        <v>5.0076472834204369</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+        <v>5.01</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
     </row>
-    <row r="18" spans="1:15" ht="16.5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:15" ht="16.5" x14ac:dyDescent="0.6">
       <c r="A18" s="24" t="s">
         <v>8</v>
       </c>
       <c r="B18" s="25"/>
       <c r="J18" s="18">
         <f>H16</f>
-        <v>5.0076472834204369</v>
+        <v>5.01</v>
       </c>
       <c r="K18" s="21">
         <v>7.2999999999999995E-2</v>
@@ -1138,7 +1043,7 @@
         <v>7.6999999999999999E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A19" s="10" t="s">
         <v>9</v>
       </c>
@@ -1150,71 +1055,71 @@
       </c>
       <c r="K19" s="6">
         <f t="dataTable" ref="K19:O23" dt2D="1" dtr="1" r1="E3" r2="B11"/>
-        <v>4.7398388485848475</v>
+        <v>5.01</v>
       </c>
       <c r="L19" s="6">
-        <v>4.7383655606256418</v>
+        <v>5.01</v>
       </c>
       <c r="M19" s="6">
-        <v>4.7368991156113864</v>
+        <v>5.01</v>
       </c>
       <c r="N19" s="6">
-        <v>4.7354394754375733</v>
+        <v>5.01</v>
       </c>
       <c r="O19" s="6">
-        <v>4.7339866022470103</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>5.01</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A20" s="12" t="s">
         <v>10</v>
       </c>
       <c r="B20" s="13">
         <f>B16-B19</f>
-        <v>9279.170416178069</v>
+        <v>9283</v>
       </c>
       <c r="J20" s="21">
         <v>2.4E-2</v>
       </c>
       <c r="K20" s="6">
-        <v>4.8725585386873238</v>
+        <v>5.01</v>
       </c>
       <c r="L20" s="6">
-        <v>4.8710852507281173</v>
+        <v>5.01</v>
       </c>
       <c r="M20" s="6">
-        <v>4.8696188057138619</v>
+        <v>5.01</v>
       </c>
       <c r="N20" s="6">
-        <v>4.8681591655400487</v>
+        <v>5.01</v>
       </c>
       <c r="O20" s="6">
-        <v>4.8667062923494857</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+        <v>5.01</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="J21" s="21">
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="K21" s="6">
-        <v>5.0105870163938979</v>
+        <v>5.01</v>
       </c>
       <c r="L21" s="6">
-        <v>5.0091137284346923</v>
+        <v>5.01</v>
       </c>
       <c r="M21" s="6">
-        <v>5.0076472834204369</v>
+        <v>5.01</v>
       </c>
       <c r="N21" s="6">
-        <v>5.0061876432466237</v>
+        <v>5.01</v>
       </c>
       <c r="O21" s="6">
-        <v>5.0047347700560607</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" ht="16.5" x14ac:dyDescent="0.45">
+        <v>5.01</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="16.5" x14ac:dyDescent="0.6">
       <c r="A22" s="26" t="s">
         <v>12</v>
       </c>
@@ -1223,22 +1128,22 @@
         <v>2.6000000000000002E-2</v>
       </c>
       <c r="K22" s="6">
-        <v>5.1542493095170698</v>
+        <v>5.01</v>
       </c>
       <c r="L22" s="6">
-        <v>5.1527760215578633</v>
+        <v>5.01</v>
       </c>
       <c r="M22" s="6">
-        <v>5.1513095765436079</v>
+        <v>5.01</v>
       </c>
       <c r="N22" s="6">
-        <v>5.1498499363697947</v>
+        <v>5.01</v>
       </c>
       <c r="O22" s="6">
-        <v>5.1483970631792317</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
+        <v>5.01</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A23" s="3" t="s">
         <v>13</v>
       </c>
@@ -1249,34 +1154,33 @@
         <v>2.7000000000000003E-2</v>
       </c>
       <c r="K23" s="6">
-        <v>5.3038975315203709</v>
+        <v>5.01</v>
       </c>
       <c r="L23" s="6">
-        <v>5.3024242435611653</v>
+        <v>5.01</v>
       </c>
       <c r="M23" s="6">
-        <v>5.3009577985469098</v>
+        <v>5.01</v>
       </c>
       <c r="N23" s="6">
-        <v>5.2994981583730967</v>
+        <v>5.01</v>
       </c>
       <c r="O23" s="6">
-        <v>5.2980452851825337</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>5.01</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A24" s="12" t="s">
         <v>11</v>
       </c>
       <c r="B24" s="14">
-        <f>B20/B23</f>
-        <v>5.0076472834204369</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+        <v>5.01</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="L25" s="6"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.45">
       <c r="L26" s="6"/>
     </row>
   </sheetData>
@@ -1289,7 +1193,519 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AA70213-F3C2-4630-B34B-890FBA1251F3}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E4"/>
+    </sheetView>
+    <sheetView workbookViewId="1">
+      <selection activeCell="G24" sqref="G24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="26.06640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.06640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2">
+        <v>4.2</v>
+      </c>
+      <c r="C2">
+        <v>1.8</v>
+      </c>
+      <c r="D2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3">
+        <v>3.5</v>
+      </c>
+      <c r="C3">
+        <v>1.5</v>
+      </c>
+      <c r="D3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4">
+        <v>4.5</v>
+      </c>
+      <c r="C4">
+        <v>1.8</v>
+      </c>
+      <c r="D4">
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5">
+        <v>4.7</v>
+      </c>
+      <c r="C5">
+        <v>0.6</v>
+      </c>
+      <c r="D5">
+        <v>5.3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5393FF5A-4A4F-4A89-8BF1-96F397853368}">
+  <dimension ref="A1:O26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
+    </sheetView>
+    <sheetView topLeftCell="A4" zoomScale="88" workbookViewId="1">
+      <selection activeCell="D20" sqref="D20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="19.796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.06640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1">
+        <v>2025</v>
+      </c>
+      <c r="C1">
+        <v>2026</v>
+      </c>
+      <c r="D1">
+        <v>2027</v>
+      </c>
+      <c r="E1">
+        <v>2028</v>
+      </c>
+      <c r="F1">
+        <v>2029</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1">
+        <v>552</v>
+      </c>
+      <c r="C2" s="1">
+        <v>641</v>
+      </c>
+      <c r="D2" s="1">
+        <v>870</v>
+      </c>
+      <c r="E2" s="1">
+        <v>973</v>
+      </c>
+      <c r="F2" s="1">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="15">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="C3" s="15">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="D3" s="15">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="E3" s="15">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="F3" s="15">
+        <v>7.4999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5">
+        <f>B2/(1+B3)^B4</f>
+        <v>513.48837209302326</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ref="C5:F5" si="0">C2/(1+C3)^C4</f>
+        <v>554.67820443482969</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>700.31569547335459</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>728.58291547241276</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>606.70256877695113</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="16.5" x14ac:dyDescent="0.6">
+      <c r="A9" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="23"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="4">
+        <f>F2</f>
+        <v>871</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A11" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" s="5">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="6">
+        <f>B10*(1+B11)</f>
+        <v>892.77499999999998</v>
+      </c>
+      <c r="F12" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="H12" s="16">
+        <f>B16</f>
+        <v>15541.170416178069</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A13" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="4">
+        <f>B12/(F3-B11)</f>
+        <v>17855.5</v>
+      </c>
+      <c r="F13" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="G13" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="H13" s="16">
+        <f>B19</f>
+        <v>6262</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A14" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="4">
+        <f>B13/(1+F3)^F4</f>
+        <v>12437.402659927498</v>
+      </c>
+      <c r="F14" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="H14" s="16">
+        <f>B20</f>
+        <v>9279.170416178069</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A15" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="4">
+        <f>SUM(B5:F5)</f>
+        <v>3103.7677562505714</v>
+      </c>
+      <c r="F15" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="G15" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="H15" s="16">
+        <f>B23</f>
+        <v>1853</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A16" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="8">
+        <f>SUM(B14:B15)</f>
+        <v>15541.170416178069</v>
+      </c>
+      <c r="F16" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="G16" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="H16" s="18">
+        <f>B24</f>
+        <v>5.0076472834204369</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+    </row>
+    <row r="18" spans="1:15" ht="16.5" x14ac:dyDescent="0.6">
+      <c r="A18" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="25"/>
+      <c r="J18" s="18">
+        <f>H16</f>
+        <v>5.0076472834204369</v>
+      </c>
+      <c r="K18" s="21">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="L18" s="21">
+        <v>7.400000000000001E-2</v>
+      </c>
+      <c r="M18" s="21">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="N18" s="21">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="O18" s="21">
+        <v>7.6999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A19" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="11">
+        <v>6262</v>
+      </c>
+      <c r="J19" s="21">
+        <v>2.3E-2</v>
+      </c>
+      <c r="K19" s="6">
+        <f t="dataTable" ref="K19:O23" dt2D="1" dtr="1" r1="E3" r2="B11"/>
+        <v>4.7398388485848475</v>
+      </c>
+      <c r="L19" s="6">
+        <v>4.7383655606256418</v>
+      </c>
+      <c r="M19" s="6">
+        <v>4.7368991156113864</v>
+      </c>
+      <c r="N19" s="6">
+        <v>4.7354394754375733</v>
+      </c>
+      <c r="O19" s="6">
+        <v>4.7339866022470103</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A20" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="13">
+        <f>B16-B19</f>
+        <v>9279.170416178069</v>
+      </c>
+      <c r="J20" s="21">
+        <v>2.4E-2</v>
+      </c>
+      <c r="K20" s="6">
+        <v>4.8725585386873238</v>
+      </c>
+      <c r="L20" s="6">
+        <v>4.8710852507281173</v>
+      </c>
+      <c r="M20" s="6">
+        <v>4.8696188057138619</v>
+      </c>
+      <c r="N20" s="6">
+        <v>4.8681591655400487</v>
+      </c>
+      <c r="O20" s="6">
+        <v>4.8667062923494857</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="J21" s="21">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="K21" s="6">
+        <v>5.0105870163938979</v>
+      </c>
+      <c r="L21" s="6">
+        <v>5.0091137284346923</v>
+      </c>
+      <c r="M21" s="6">
+        <v>5.0076472834204369</v>
+      </c>
+      <c r="N21" s="6">
+        <v>5.0061876432466237</v>
+      </c>
+      <c r="O21" s="6">
+        <v>5.0047347700560607</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="16.5" x14ac:dyDescent="0.6">
+      <c r="A22" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="27"/>
+      <c r="J22" s="21">
+        <v>2.6000000000000002E-2</v>
+      </c>
+      <c r="K22" s="6">
+        <v>5.1542493095170698</v>
+      </c>
+      <c r="L22" s="6">
+        <v>5.1527760215578633</v>
+      </c>
+      <c r="M22" s="6">
+        <v>5.1513095765436079</v>
+      </c>
+      <c r="N22" s="6">
+        <v>5.1498499363697947</v>
+      </c>
+      <c r="O22" s="6">
+        <v>5.1483970631792317</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A23" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="9">
+        <v>1853</v>
+      </c>
+      <c r="J23" s="21">
+        <v>2.7000000000000003E-2</v>
+      </c>
+      <c r="K23" s="6">
+        <v>5.3038975315203709</v>
+      </c>
+      <c r="L23" s="6">
+        <v>5.3024242435611653</v>
+      </c>
+      <c r="M23" s="6">
+        <v>5.3009577985469098</v>
+      </c>
+      <c r="N23" s="6">
+        <v>5.2994981583730967</v>
+      </c>
+      <c r="O23" s="6">
+        <v>5.2980452851825337</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A24" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" s="14">
+        <f>B20/B23</f>
+        <v>5.0076472834204369</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="L25" s="6"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="L26" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A22:B22"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89343CA2-2E31-49A3-989D-0233F24AEB06}">
   <dimension ref="A1:Q20"/>
   <sheetViews>
@@ -1300,17 +1716,17 @@
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="23.1796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.08984375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.81640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.81640625" customWidth="1"/>
-    <col min="15" max="15" width="10.6328125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.19921875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.06640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.796875" customWidth="1"/>
+    <col min="15" max="15" width="10.59765625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A1" s="28" t="s">
         <v>19</v>
       </c>
@@ -1329,7 +1745,7 @@
         <v>9.1999999999999993</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
         <v>22</v>
       </c>
@@ -1349,7 +1765,7 @@
         <v>6.86</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1366,7 +1782,7 @@
         <v>62.47</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1389,7 +1805,7 @@
         <v>7.3</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J5" t="s">
         <v>49</v>
       </c>
@@ -1400,7 +1816,7 @@
         <v>1.85</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A6" s="28" t="s">
         <v>24</v>
       </c>
@@ -1419,7 +1835,7 @@
         <v>1.59</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -1436,7 +1852,7 @@
         <v>9.4</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
         <v>29</v>
       </c>
@@ -1456,7 +1872,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -1470,7 +1886,7 @@
         <v>1055</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -1484,7 +1900,7 @@
         <v>1084</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -1501,7 +1917,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.45">
       <c r="K12" t="s">
         <v>56</v>
       </c>
@@ -1524,7 +1940,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A13" s="28" t="s">
         <v>32</v>
       </c>
@@ -1538,7 +1954,7 @@
         <v>13.97</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -1570,7 +1986,7 @@
         <v>3.1034248079034032</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>34</v>
       </c>
@@ -1605,12 +2021,12 @@
         <v>4.6269224123034389</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -1636,7 +2052,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>36</v>
       </c>
@@ -1647,7 +2063,7 @@
         <v>13.97</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J19" t="s">
         <v>48</v>
       </c>
@@ -1676,7 +2092,7 @@
         <v>6.3100109769484085</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J20" t="s">
         <v>52</v>
       </c>

</xml_diff>

<commit_message>
Updated graph, updated txt file
</commit_message>
<xml_diff>
--- a/DCF Excel/DCF.xlsx
+++ b/DCF Excel/DCF.xlsx
@@ -8,10 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\niamh\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FA13E8F-12F1-49A0-BC97-E162CB410918}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{090EA610-2A33-49E2-AF67-D4796EE1B99A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="2" xr2:uid="{02DDE7C9-D2BD-4C78-80A5-9CD0E38E0A7F}"/>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{A124F699-F544-4474-B589-20D8B152A358}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{02DDE7C9-D2BD-4C78-80A5-9CD0E38E0A7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="5" r:id="rId1"/>
@@ -229,8 +228,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -401,7 +401,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -424,6 +424,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -445,7 +446,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -783,11 +789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D395B51-2BB7-401F-ABD9-7600F8F8CFD4}">
   <dimension ref="A1:O26"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
-    </sheetView>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="88" workbookViewId="1">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -903,10 +906,10 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="16.5" x14ac:dyDescent="0.6">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="23"/>
+      <c r="B9" s="24"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10" s="3" t="s">
@@ -928,8 +931,8 @@
       <c r="A12" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="29">
-        <v>893</v>
+      <c r="B12" s="22">
+        <v>892.8</v>
       </c>
       <c r="F12" s="19" t="s">
         <v>6</v>
@@ -939,7 +942,7 @@
       </c>
       <c r="H12" s="16">
         <f>B16</f>
-        <v>15545</v>
+        <v>15541.2</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.45">
@@ -947,7 +950,7 @@
         <v>3</v>
       </c>
       <c r="B13" s="4">
-        <v>17860</v>
+        <v>17855.5</v>
       </c>
       <c r="F13" s="19" t="s">
         <v>36</v>
@@ -965,7 +968,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="4">
-        <v>12441</v>
+        <v>12437.4</v>
       </c>
       <c r="F14" s="19" t="s">
         <v>10</v>
@@ -975,7 +978,7 @@
       </c>
       <c r="H14" s="16">
         <f>B20</f>
-        <v>9283</v>
+        <v>9279.2000000000007</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.45">
@@ -983,7 +986,7 @@
         <v>5</v>
       </c>
       <c r="B15" s="4">
-        <v>3104</v>
+        <v>3103.8</v>
       </c>
       <c r="F15" s="19" t="s">
         <v>38</v>
@@ -1001,7 +1004,7 @@
         <v>6</v>
       </c>
       <c r="B16" s="8">
-        <v>15545</v>
+        <v>15541.2</v>
       </c>
       <c r="F16" s="19" t="s">
         <v>39</v>
@@ -1019,10 +1022,10 @@
       <c r="B17" s="2"/>
     </row>
     <row r="18" spans="1:15" ht="16.5" x14ac:dyDescent="0.6">
-      <c r="A18" s="24" t="s">
+      <c r="A18" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="25"/>
+      <c r="B18" s="26"/>
       <c r="J18" s="18">
         <f>H16</f>
         <v>5.01</v>
@@ -1075,8 +1078,7 @@
         <v>10</v>
       </c>
       <c r="B20" s="13">
-        <f>B16-B19</f>
-        <v>9283</v>
+        <v>9279.2000000000007</v>
       </c>
       <c r="J20" s="21">
         <v>2.4E-2</v>
@@ -1120,10 +1122,10 @@
       </c>
     </row>
     <row r="22" spans="1:15" ht="16.5" x14ac:dyDescent="0.6">
-      <c r="A22" s="26" t="s">
+      <c r="A22" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="B22" s="27"/>
+      <c r="B22" s="28"/>
       <c r="J22" s="21">
         <v>2.6000000000000002E-2</v>
       </c>
@@ -1200,9 +1202,6 @@
     <sheetView workbookViewId="0">
       <selection sqref="A1:E4"/>
     </sheetView>
-    <sheetView workbookViewId="1">
-      <selection activeCell="G24" sqref="G24"/>
-    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -1288,11 +1287,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5393FF5A-4A4F-4A89-8BF1-96F397853368}">
   <dimension ref="A1:O26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
-    </sheetView>
-    <sheetView topLeftCell="A4" zoomScale="88" workbookViewId="1">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView topLeftCell="A2" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1408,16 +1404,16 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="16.5" x14ac:dyDescent="0.6">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="23"/>
+      <c r="B9" s="24"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="30">
         <f>F2</f>
         <v>871</v>
       </c>
@@ -1426,7 +1422,7 @@
       <c r="A11" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="31">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -1434,7 +1430,7 @@
       <c r="A12" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="32">
         <f>B10*(1+B11)</f>
         <v>892.77499999999998</v>
       </c>
@@ -1453,7 +1449,7 @@
       <c r="A13" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="30">
         <f>B12/(F3-B11)</f>
         <v>17855.5</v>
       </c>
@@ -1472,7 +1468,7 @@
       <c r="A14" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14" s="30">
         <f>B13/(1+F3)^F4</f>
         <v>12437.402659927498</v>
       </c>
@@ -1491,7 +1487,7 @@
       <c r="A15" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="30">
         <f>SUM(B5:F5)</f>
         <v>3103.7677562505714</v>
       </c>
@@ -1510,7 +1506,7 @@
       <c r="A16" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="8">
+      <c r="B16" s="33">
         <f>SUM(B14:B15)</f>
         <v>15541.170416178069</v>
       </c>
@@ -1530,10 +1526,10 @@
       <c r="B17" s="2"/>
     </row>
     <row r="18" spans="1:15" ht="16.5" x14ac:dyDescent="0.6">
-      <c r="A18" s="24" t="s">
+      <c r="A18" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="25"/>
+      <c r="B18" s="26"/>
       <c r="J18" s="18">
         <f>H16</f>
         <v>5.0076472834204369</v>
@@ -1558,7 +1554,7 @@
       <c r="A19" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="11">
+      <c r="B19" s="34">
         <v>6262</v>
       </c>
       <c r="J19" s="21">
@@ -1585,7 +1581,7 @@
       <c r="A20" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="13">
+      <c r="B20" s="35">
         <f>B16-B19</f>
         <v>9279.170416178069</v>
       </c>
@@ -1631,10 +1627,10 @@
       </c>
     </row>
     <row r="22" spans="1:15" ht="16.5" x14ac:dyDescent="0.6">
-      <c r="A22" s="26" t="s">
+      <c r="A22" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="B22" s="27"/>
+      <c r="B22" s="28"/>
       <c r="J22" s="21">
         <v>2.6000000000000002E-2</v>
       </c>
@@ -1658,7 +1654,7 @@
       <c r="A23" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="9">
+      <c r="B23" s="31">
         <v>1853</v>
       </c>
       <c r="J23" s="21">
@@ -1712,9 +1708,6 @@
     <sheetView topLeftCell="E1" zoomScale="82" workbookViewId="0">
       <selection activeCell="O9" sqref="O9"/>
     </sheetView>
-    <sheetView zoomScale="66" workbookViewId="1">
-      <selection activeCell="I13" sqref="I13"/>
-    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -1727,11 +1720,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
       <c r="J1" t="s">
         <v>51</v>
       </c>
@@ -1817,11 +1810,11 @@
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
       <c r="J6" t="s">
         <v>50</v>
       </c>
@@ -1941,12 +1934,12 @@
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A13" s="28" t="s">
+      <c r="A13" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="28"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
       <c r="J13" t="s">
         <v>46</v>
       </c>

</xml_diff>